<commit_message>
Speichern der End-Ergebnisse in Excel
</commit_message>
<xml_diff>
--- a/src_evaluation/evaluation.xlsx
+++ b/src_evaluation/evaluation.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="mnist_fashion" sheetId="1" r:id="rId1"/>
     <sheet name="mnist_digits" sheetId="2" r:id="rId2"/>
     <sheet name="cifar10" sheetId="3" r:id="rId3"/>
+    <sheet name="mnist_fashion_small" sheetId="6" r:id="rId4"/>
+    <sheet name="mnist_digits_small" sheetId="4" r:id="rId5"/>
+    <sheet name="cifar10_small" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="7">
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>KNN_size</t>
+  </si>
   <si>
     <t>small</t>
   </si>
@@ -27,49 +36,10 @@
     <t>big</t>
   </si>
   <si>
-    <t>RandomSearch</t>
+    <t>GA</t>
   </si>
   <si>
-    <t>Genetic Algortihmen</t>
-  </si>
-  <si>
-    <t>Iterations</t>
-  </si>
-  <si>
-    <t>KNN size</t>
-  </si>
-  <si>
-    <t>KNN_size</t>
-  </si>
-  <si>
-    <t>fff</t>
-  </si>
-  <si>
-    <t>Durchäufe</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>ccc</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>eee</t>
-  </si>
-  <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>hhh</t>
-  </si>
-  <si>
-    <t>jjj</t>
+    <t>RS</t>
   </si>
 </sst>
 </file>
@@ -105,10 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -410,146 +379,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>50</v>
+      </c>
+      <c r="D1">
+        <v>50</v>
+      </c>
+      <c r="E1">
+        <v>250</v>
+      </c>
+      <c r="F1">
+        <v>250</v>
+      </c>
+      <c r="G1">
+        <v>250</v>
+      </c>
+      <c r="H1">
+        <v>500</v>
+      </c>
+      <c r="I1">
+        <v>500</v>
+      </c>
+      <c r="J1">
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>50</v>
-      </c>
-      <c r="C2" s="1">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1">
-        <v>250</v>
-      </c>
-      <c r="F2" s="1">
-        <v>250</v>
-      </c>
-      <c r="G2" s="1">
-        <v>250</v>
-      </c>
-      <c r="H2" s="1">
-        <v>750</v>
-      </c>
-      <c r="I2" s="1">
-        <v>750</v>
-      </c>
-      <c r="J2" s="1">
-        <v>750</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -558,86 +477,86 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1">
-        <v>50</v>
-      </c>
-      <c r="C1" s="1">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1">
-        <v>50</v>
-      </c>
-      <c r="E1" s="1">
-        <v>250</v>
-      </c>
-      <c r="F1" s="1">
-        <v>250</v>
-      </c>
-      <c r="G1" s="1">
-        <v>250</v>
-      </c>
-      <c r="H1" s="1">
-        <v>750</v>
-      </c>
-      <c r="I1" s="1">
-        <v>750</v>
-      </c>
-      <c r="J1" s="1">
-        <v>750</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>50</v>
+      </c>
+      <c r="D1">
+        <v>50</v>
+      </c>
+      <c r="E1">
+        <v>250</v>
+      </c>
+      <c r="F1">
+        <v>250</v>
+      </c>
+      <c r="G1">
+        <v>250</v>
+      </c>
+      <c r="H1">
+        <v>500</v>
+      </c>
+      <c r="I1">
+        <v>500</v>
+      </c>
+      <c r="J1">
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -647,45 +566,376 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1">
-        <v>50</v>
-      </c>
-      <c r="C1" s="1">
-        <v>250</v>
-      </c>
-      <c r="D1" s="1">
-        <v>750</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>50</v>
+      </c>
+      <c r="D1">
+        <v>50</v>
+      </c>
+      <c r="E1">
+        <v>250</v>
+      </c>
+      <c r="F1">
+        <v>250</v>
+      </c>
+      <c r="G1">
+        <v>250</v>
+      </c>
+      <c r="H1">
+        <v>500</v>
+      </c>
+      <c r="I1">
+        <v>500</v>
+      </c>
+      <c r="J1">
+        <v>500</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1">
+        <v>250</v>
+      </c>
+      <c r="F1" s="1">
+        <v>250</v>
+      </c>
+      <c r="G1" s="1">
+        <v>250</v>
+      </c>
+      <c r="H1" s="1">
+        <v>500</v>
+      </c>
+      <c r="I1" s="1">
+        <v>500</v>
+      </c>
+      <c r="J1" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1">
+        <v>250</v>
+      </c>
+      <c r="F1" s="1">
+        <v>250</v>
+      </c>
+      <c r="G1" s="1">
+        <v>250</v>
+      </c>
+      <c r="H1" s="1">
+        <v>500</v>
+      </c>
+      <c r="I1" s="1">
+        <v>500</v>
+      </c>
+      <c r="J1" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1">
+        <v>250</v>
+      </c>
+      <c r="F1" s="1">
+        <v>250</v>
+      </c>
+      <c r="G1" s="1">
+        <v>250</v>
+      </c>
+      <c r="H1" s="1">
+        <v>500</v>
+      </c>
+      <c r="I1" s="1">
+        <v>500</v>
+      </c>
+      <c r="J1" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>